<commit_message>
Se acutalizó el informe
</commit_message>
<xml_diff>
--- a/Informe_Placas_Validadas_Tenencia_Aux-15-21.xlsx
+++ b/Informe_Placas_Validadas_Tenencia_Aux-15-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jodopevi\GitHub\Validacion_Placas_Tenencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205F307F-1D50-4392-95A4-3F4230CB81DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA193A29-F7AF-4728-B80D-A1A56F47AB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16776" xr2:uid="{6274E1BB-F630-4362-BD7C-8E4681F5E052}"/>
   </bookViews>
@@ -172,9 +172,9 @@
   <colors>
     <mruColors>
       <color rgb="FF10312B"/>
+      <color rgb="FF6F7271"/>
       <color rgb="FFDDC9A3"/>
       <color rgb="FF691C20"/>
-      <color rgb="FF6F7271"/>
       <color rgb="FF98989A"/>
       <color rgb="FFBC955C"/>
       <color rgb="FF235B4E"/>
@@ -517,7 +517,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -544,6 +543,7 @@
                   <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="inEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -561,7 +561,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -588,6 +587,7 @@
                   <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="inEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -605,7 +605,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -620,7 +619,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="700" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="DDC9A3"/>
                       </a:solidFill>
@@ -632,6 +631,7 @@
                   <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="inEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -651,11 +651,10 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7149999999999996E-3"/>
-                  <c:y val="-0.18191450916936353"/>
+                  <c:x val="-1.7610300789038479E-2"/>
+                  <c:y val="-0.19115548714055769"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -670,7 +669,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="98989A"/>
                       </a:solidFill>
@@ -701,11 +700,10 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.0866944444444445E-2"/>
-                  <c:y val="-0.17493284789644012"/>
+                  <c:x val="-6.8431464424976397E-3"/>
+                  <c:y val="-0.18532876776766871"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -720,7 +718,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="98989A"/>
                       </a:solidFill>
@@ -751,11 +749,10 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.8805555555555561E-4"/>
-                  <c:y val="-0.14268500539374326"/>
+                  <c:x val="2.3026978721577599E-3"/>
+                  <c:y val="-0.15656391981171097"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -770,7 +767,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="98989A"/>
                       </a:solidFill>
@@ -814,7 +811,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="10312B"/>
                       </a:solidFill>
@@ -859,7 +856,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="10312B"/>
                       </a:solidFill>
@@ -904,7 +901,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="98989A"/>
                       </a:solidFill>
@@ -934,40 +931,9 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:numFmt formatCode="0.0%" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="bg1"/>
-                      </a:solidFill>
-                      <a:latin typeface="Source Sans Pro" panose="020B0503030403020204" pitchFamily="34" charset="0"/>
-                      <a:ea typeface="Source Sans Pro" panose="020B0503030403020204" pitchFamily="34" charset="0"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-MX"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000014-1283-0644-A01D-0FB135BC3434}"/>
                 </c:ext>
@@ -1000,11 +966,25 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="6F7271"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
@@ -1145,9 +1125,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35014325386345269"/>
+          <c:x val="0.34483325718997276"/>
           <c:y val="0.15942610482197966"/>
-          <c:w val="0.64985674613654731"/>
+          <c:w val="0.65516674281002718"/>
           <c:h val="0.83445003018026565"/>
         </c:manualLayout>
       </c:layout>

</xml_diff>